<commit_message>
Uses new <time.h> from latest cc65
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - FuckBench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9B90CB-DF3F-4154-97D2-91565D203F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A602E3-9325-41FE-8FC1-C012B7D6AD85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="0" windowWidth="13485" windowHeight="15480" xr2:uid="{9ABD8A58-D3BB-4318-B9A1-DF7273AC6AAF}"/>
   </bookViews>
@@ -431,10 +431,18 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">

</xml_diff>